<commit_message>
Task 2 - Complete
Added Lexeme Classes and Regex
</commit_message>
<xml_diff>
--- a/A21/A21-Task1.xlsx
+++ b/A21/A21-Task1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Github\CST8152\ACW24_CST8152\A21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDrive\Desktop\A21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B1B4ED2-732D-4886-BAA6-F739977A5F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753BBEFB-97A8-4C4D-B78B-5A62699424B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DDC880CA-115F-4A2E-83FE-A9474966E49D}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{DDC880CA-115F-4A2E-83FE-A9474966E49D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Task 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Task 1 - Language Symbols" sheetId="1" r:id="rId1"/>
+    <sheet name="Task 2 - Lexemes &amp; RE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="135">
   <si>
     <t>KEYWORDS</t>
   </si>
@@ -363,13 +364,403 @@
   </si>
   <si>
     <t>bool = true, false</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,6 +775,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -406,25 +811,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,117 +1152,117 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="b">
+      <c r="A3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="5" t="b">
+      <c r="G4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -909,7 +1313,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -978,7 +1382,7 @@
       <c r="F13" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1001,7 +1405,7 @@
       <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1024,12 +1428,12 @@
       <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1047,7 +1451,7 @@
       <c r="F16" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1069,25 +1473,25 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="7"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1097,7 +1501,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1127,7 +1531,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1142,107 +1546,107 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G44" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J44" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="b">
+      <c r="A45" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="G45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J45" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K45" s="5" t="s">
+      <c r="K45" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G46" s="5" t="b">
+      <c r="G46" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J46" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="K46" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1369,6 +1773,154 @@
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F31117-FE1A-41B9-B61E-D6B46969B018}">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>